<commit_message>
removes category from rocprof comparison data for further simplification
</commit_message>
<xml_diff>
--- a/tests/traces/compare_test/reference/compare_56ch_rank7_across_threads.xlsx
+++ b/tests/traces/compare_test/reference/compare_56ch_rank7_across_threads.xlsx
@@ -605,7 +605,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R47"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -676,32 +676,22 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>256thread::Category</t>
+          <t>512thread::Count</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>512thread::Count</t>
+          <t>512thread::Mean Kernel Time (µs)</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>512thread::Mean Kernel Time (µs)</t>
+          <t>512thread::Percentage (%)</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>512thread::Percentage (%)</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
           <t>512thread::Total Kernel Time (ms)</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>512thread::Category</t>
         </is>
       </c>
     </row>
@@ -744,27 +734,17 @@
       <c r="L2" t="n">
         <v>27018592.547</v>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>COMM</t>
-        </is>
+      <c r="M2" t="n">
+        <v>270</v>
       </c>
       <c r="N2" t="n">
-        <v>270</v>
+        <v>42028966.12962963</v>
       </c>
       <c r="O2" t="n">
-        <v>42028966.12962963</v>
+        <v>72.0850230522221</v>
       </c>
       <c r="P2" t="n">
-        <v>72.0850230522221</v>
-      </c>
-      <c r="Q2" t="n">
         <v>11347820.855</v>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>COMM</t>
-        </is>
       </c>
     </row>
     <row r="3">
@@ -806,27 +786,17 @@
       <c r="L3" t="n">
         <v>681272.884</v>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Elementwise</t>
-        </is>
+      <c r="M3" t="n">
+        <v>10247</v>
       </c>
       <c r="N3" t="n">
-        <v>10247</v>
+        <v>67153.60466477994</v>
       </c>
       <c r="O3" t="n">
-        <v>67153.60466477994</v>
+        <v>4.371179455023123</v>
       </c>
       <c r="P3" t="n">
-        <v>4.371179455023123</v>
-      </c>
-      <c r="Q3" t="n">
         <v>688122.987</v>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>Elementwise</t>
-        </is>
       </c>
     </row>
     <row r="4">
@@ -868,27 +838,17 @@
       <c r="L4" t="n">
         <v>478633.788</v>
       </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>Elementwise</t>
-        </is>
+      <c r="M4" t="n">
+        <v>2060</v>
       </c>
       <c r="N4" t="n">
-        <v>2060</v>
+        <v>233816.7684466019</v>
       </c>
       <c r="O4" t="n">
-        <v>233816.7684466019</v>
+        <v>3.059676034650171</v>
       </c>
       <c r="P4" t="n">
-        <v>3.059676034650171</v>
-      </c>
-      <c r="Q4" t="n">
         <v>481662.543</v>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>Elementwise</t>
-        </is>
       </c>
     </row>
     <row r="5">
@@ -930,27 +890,17 @@
       <c r="L5" t="n">
         <v>431185.19</v>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M5" t="n">
+        <v>200</v>
       </c>
       <c r="N5" t="n">
-        <v>200</v>
+        <v>2212016.62</v>
       </c>
       <c r="O5" t="n">
-        <v>2212016.62</v>
+        <v>2.810288796096762</v>
       </c>
       <c r="P5" t="n">
-        <v>2.810288796096762</v>
-      </c>
-      <c r="Q5" t="n">
         <v>442403.324</v>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="6">
@@ -992,27 +942,17 @@
       <c r="L6" t="n">
         <v>369397.203</v>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
+      <c r="M6" t="n">
+        <v>620</v>
       </c>
       <c r="N6" t="n">
-        <v>620</v>
+        <v>611653.5016129032</v>
       </c>
       <c r="O6" t="n">
-        <v>611653.5016129032</v>
+        <v>2.408960763728753</v>
       </c>
       <c r="P6" t="n">
-        <v>2.408960763728753</v>
-      </c>
-      <c r="Q6" t="n">
         <v>379225.171</v>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
       </c>
     </row>
     <row r="7">
@@ -1054,27 +994,17 @@
       <c r="L7" t="n">
         <v>306416.952</v>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
+      <c r="M7" t="n">
+        <v>610</v>
       </c>
       <c r="N7" t="n">
-        <v>610</v>
+        <v>494612.062295082</v>
       </c>
       <c r="O7" t="n">
-        <v>494612.062295082</v>
+        <v>1.916580693729443</v>
       </c>
       <c r="P7" t="n">
-        <v>1.916580693729443</v>
-      </c>
-      <c r="Q7" t="n">
         <v>301713.358</v>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
       </c>
     </row>
     <row r="8">
@@ -1116,27 +1046,17 @@
       <c r="L8" t="n">
         <v>269720.129</v>
       </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
+      <c r="M8" t="n">
+        <v>410</v>
       </c>
       <c r="N8" t="n">
-        <v>410</v>
+        <v>674966.3634146341</v>
       </c>
       <c r="O8" t="n">
-        <v>674966.3634146341</v>
+        <v>1.757917776465423</v>
       </c>
       <c r="P8" t="n">
-        <v>1.757917776465423</v>
-      </c>
-      <c r="Q8" t="n">
         <v>276736.209</v>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
       </c>
     </row>
     <row r="9">
@@ -1178,27 +1098,17 @@
       <c r="L9" t="n">
         <v>223026.67</v>
       </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
+      <c r="M9" t="n">
+        <v>200</v>
       </c>
       <c r="N9" t="n">
-        <v>200</v>
+        <v>1136174.96</v>
       </c>
       <c r="O9" t="n">
-        <v>1136174.96</v>
+        <v>1.443470058779977</v>
       </c>
       <c r="P9" t="n">
-        <v>1.443470058779977</v>
-      </c>
-      <c r="Q9" t="n">
         <v>227234.992</v>
-      </c>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
       </c>
     </row>
     <row r="10">
@@ -1240,27 +1150,17 @@
       <c r="L10" t="n">
         <v>209579.213</v>
       </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>Attention</t>
-        </is>
+      <c r="M10" t="n">
+        <v>200</v>
       </c>
       <c r="N10" t="n">
-        <v>200</v>
+        <v>1063244.1</v>
       </c>
       <c r="O10" t="n">
-        <v>1063244.1</v>
+        <v>1.35081398337142</v>
       </c>
       <c r="P10" t="n">
-        <v>1.35081398337142</v>
-      </c>
-      <c r="Q10" t="n">
         <v>212648.82</v>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>Attention</t>
-        </is>
       </c>
     </row>
     <row r="11">
@@ -1302,27 +1202,17 @@
       <c r="L11" t="n">
         <v>202623.633</v>
       </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
+      <c r="M11" t="n">
+        <v>420</v>
       </c>
       <c r="N11" t="n">
-        <v>420</v>
+        <v>480581.6952380952</v>
       </c>
       <c r="O11" t="n">
-        <v>480581.6952380952</v>
+        <v>1.282180259046741</v>
       </c>
       <c r="P11" t="n">
-        <v>1.282180259046741</v>
-      </c>
-      <c r="Q11" t="n">
         <v>201844.312</v>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
       </c>
     </row>
     <row r="12">
@@ -1364,27 +1254,17 @@
       <c r="L12" t="n">
         <v>165885.894</v>
       </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
+      <c r="M12" t="n">
+        <v>200</v>
       </c>
       <c r="N12" t="n">
-        <v>200</v>
+        <v>820126.465</v>
       </c>
       <c r="O12" t="n">
-        <v>820126.465</v>
+        <v>1.041941636031624</v>
       </c>
       <c r="P12" t="n">
-        <v>1.041941636031624</v>
-      </c>
-      <c r="Q12" t="n">
         <v>164025.293</v>
-      </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
       </c>
     </row>
     <row r="13">
@@ -1426,27 +1306,17 @@
       <c r="L13" t="n">
         <v>154533.113</v>
       </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M13" t="n">
+        <v>610</v>
       </c>
       <c r="N13" t="n">
-        <v>610</v>
+        <v>251534.7</v>
       </c>
       <c r="O13" t="n">
-        <v>251534.7</v>
+        <v>0.9746760877324054</v>
       </c>
       <c r="P13" t="n">
-        <v>0.9746760877324054</v>
-      </c>
-      <c r="Q13" t="n">
         <v>153436.167</v>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="14">
@@ -1488,27 +1358,17 @@
       <c r="L14" t="n">
         <v>127043.078</v>
       </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M14" t="n">
+        <v>410</v>
       </c>
       <c r="N14" t="n">
-        <v>410</v>
+        <v>316938.7804878049</v>
       </c>
       <c r="O14" t="n">
-        <v>316938.7804878049</v>
+        <v>0.8254519728244947</v>
       </c>
       <c r="P14" t="n">
-        <v>0.8254519728244947</v>
-      </c>
-      <c r="Q14" t="n">
         <v>129944.9</v>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="15">
@@ -1550,27 +1410,17 @@
       <c r="L15" t="n">
         <v>101327.439</v>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M15" t="n">
+        <v>1900</v>
       </c>
       <c r="N15" t="n">
-        <v>1900</v>
+        <v>45932.34789473684</v>
       </c>
       <c r="O15" t="n">
-        <v>45932.34789473684</v>
+        <v>0.5543765061478053</v>
       </c>
       <c r="P15" t="n">
-        <v>0.5543765061478053</v>
-      </c>
-      <c r="Q15" t="n">
         <v>87271.461</v>
-      </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="16">
@@ -1612,27 +1462,17 @@
       <c r="L16" t="n">
         <v>100031.527</v>
       </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M16" t="n">
+        <v>410</v>
       </c>
       <c r="N16" t="n">
-        <v>410</v>
+        <v>241858.6390243903</v>
       </c>
       <c r="O16" t="n">
-        <v>241858.6390243903</v>
+        <v>0.6299093169351425</v>
       </c>
       <c r="P16" t="n">
-        <v>0.6299093169351425</v>
-      </c>
-      <c r="Q16" t="n">
         <v>99162.042</v>
-      </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="17">
@@ -1674,27 +1514,17 @@
       <c r="L17" t="n">
         <v>99464.43700000001</v>
       </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>Reduction</t>
-        </is>
+      <c r="M17" t="n">
+        <v>910</v>
       </c>
       <c r="N17" t="n">
-        <v>910</v>
+        <v>107352.2274725275</v>
       </c>
       <c r="O17" t="n">
-        <v>107352.2274725275</v>
+        <v>0.6205617784031122</v>
       </c>
       <c r="P17" t="n">
-        <v>0.6205617784031122</v>
-      </c>
-      <c r="Q17" t="n">
         <v>97690.527</v>
-      </c>
-      <c r="R17" t="inlineStr">
-        <is>
-          <t>Reduction</t>
-        </is>
       </c>
     </row>
     <row r="18">
@@ -1736,27 +1566,17 @@
       <c r="L18" t="n">
         <v>72277.439</v>
       </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>Normalization</t>
-        </is>
+      <c r="M18" t="n">
+        <v>410</v>
       </c>
       <c r="N18" t="n">
-        <v>410</v>
+        <v>182314.9</v>
       </c>
       <c r="O18" t="n">
-        <v>182314.9</v>
+        <v>0.4748304819267489</v>
       </c>
       <c r="P18" t="n">
-        <v>0.4748304819267489</v>
-      </c>
-      <c r="Q18" t="n">
         <v>74749.109</v>
-      </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>Normalization</t>
-        </is>
       </c>
     </row>
     <row r="19">
@@ -1798,27 +1618,17 @@
       <c r="L19" t="n">
         <v>61239.326</v>
       </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>Memory</t>
-        </is>
+      <c r="M19" t="n">
+        <v>2047</v>
       </c>
       <c r="N19" t="n">
-        <v>2047</v>
+        <v>30184.96775769419</v>
       </c>
       <c r="O19" t="n">
-        <v>30184.96775769419</v>
+        <v>0.3925013271484359</v>
       </c>
       <c r="P19" t="n">
-        <v>0.3925013271484359</v>
-      </c>
-      <c r="Q19" t="n">
         <v>61788.629</v>
-      </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>Memory</t>
-        </is>
       </c>
     </row>
     <row r="20">
@@ -1860,27 +1670,17 @@
       <c r="L20" t="n">
         <v>31666.684</v>
       </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>Elementwise</t>
-        </is>
+      <c r="M20" t="n">
+        <v>200</v>
       </c>
       <c r="N20" t="n">
-        <v>200</v>
+        <v>158585.505</v>
       </c>
       <c r="O20" t="n">
-        <v>158585.505</v>
+        <v>0.2014772691558019</v>
       </c>
       <c r="P20" t="n">
-        <v>0.2014772691558019</v>
-      </c>
-      <c r="Q20" t="n">
         <v>31717.101</v>
-      </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>Elementwise</t>
-        </is>
       </c>
     </row>
     <row r="21">
@@ -1922,27 +1722,17 @@
       <c r="L21" t="n">
         <v>25684.894</v>
       </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M21" t="n">
+        <v>10</v>
       </c>
       <c r="N21" t="n">
-        <v>10</v>
+        <v>2651984.4</v>
       </c>
       <c r="O21" t="n">
-        <v>2651984.4</v>
+        <v>0.1684626141449017</v>
       </c>
       <c r="P21" t="n">
-        <v>0.1684626141449017</v>
-      </c>
-      <c r="Q21" t="n">
         <v>26519.844</v>
-      </c>
-      <c r="R21" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="22">
@@ -1984,27 +1774,17 @@
       <c r="L22" t="n">
         <v>16738.538</v>
       </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M22" t="n">
+        <v>40</v>
       </c>
       <c r="N22" t="n">
-        <v>40</v>
+        <v>427133.65</v>
       </c>
       <c r="O22" t="n">
-        <v>427133.65</v>
+        <v>0.1085316358094014</v>
       </c>
       <c r="P22" t="n">
-        <v>0.1085316358094014</v>
-      </c>
-      <c r="Q22" t="n">
         <v>17085.346</v>
-      </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="23">
@@ -2046,27 +1826,17 @@
       <c r="L23" t="n">
         <v>10891.829</v>
       </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M23" t="n">
+        <v>1864</v>
       </c>
       <c r="N23" t="n">
-        <v>1864</v>
+        <v>5644.252682403433</v>
       </c>
       <c r="O23" t="n">
-        <v>5644.252682403433</v>
+        <v>0.0668320721322159</v>
       </c>
       <c r="P23" t="n">
-        <v>0.0668320721322159</v>
-      </c>
-      <c r="Q23" t="n">
         <v>10520.887</v>
-      </c>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="24">
@@ -2108,27 +1878,17 @@
       <c r="L24" t="n">
         <v>9436.566999999999</v>
       </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>Reduction</t>
-        </is>
+      <c r="M24" t="n">
+        <v>8</v>
       </c>
       <c r="N24" t="n">
-        <v>8</v>
+        <v>24870365</v>
       </c>
       <c r="O24" t="n">
-        <v>24870365</v>
+        <v>1.263876726465772</v>
       </c>
       <c r="P24" t="n">
-        <v>1.263876726465772</v>
-      </c>
-      <c r="Q24" t="n">
         <v>198962.92</v>
-      </c>
-      <c r="R24" t="inlineStr">
-        <is>
-          <t>Reduction</t>
-        </is>
       </c>
     </row>
     <row r="25">
@@ -2170,27 +1930,17 @@
       <c r="L25" t="n">
         <v>5661.86</v>
       </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>Reduction</t>
-        </is>
+      <c r="M25" t="n">
+        <v>10</v>
       </c>
       <c r="N25" t="n">
-        <v>10</v>
+        <v>567444.9</v>
       </c>
       <c r="O25" t="n">
-        <v>567444.9</v>
+        <v>0.03604593271257265</v>
       </c>
       <c r="P25" t="n">
-        <v>0.03604593271257265</v>
-      </c>
-      <c r="Q25" t="n">
         <v>5674.449</v>
-      </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>Reduction</t>
-        </is>
       </c>
     </row>
     <row r="26">
@@ -2232,27 +1982,17 @@
       <c r="L26" t="n">
         <v>3808.624</v>
       </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M26" t="n">
+        <v>110</v>
       </c>
       <c r="N26" t="n">
-        <v>110</v>
+        <v>34347.02727272727</v>
       </c>
       <c r="O26" t="n">
-        <v>34347.02727272727</v>
+        <v>0.02400017512439688</v>
       </c>
       <c r="P26" t="n">
-        <v>0.02400017512439688</v>
-      </c>
-      <c r="Q26" t="n">
         <v>3778.173</v>
-      </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="27">
@@ -2294,27 +2034,17 @@
       <c r="L27" t="n">
         <v>3531.819</v>
       </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
+      <c r="M27" t="n">
+        <v>220</v>
       </c>
       <c r="N27" t="n">
-        <v>220</v>
+        <v>15727.71363636364</v>
       </c>
       <c r="O27" t="n">
-        <v>15727.71363636364</v>
+        <v>0.02197965364407619</v>
       </c>
       <c r="P27" t="n">
-        <v>0.02197965364407619</v>
-      </c>
-      <c r="Q27" t="n">
         <v>3460.097</v>
-      </c>
-      <c r="R27" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
       </c>
     </row>
     <row r="28">
@@ -2356,27 +2086,17 @@
       <c r="L28" t="n">
         <v>3240.931</v>
       </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
+      <c r="M28" t="n">
+        <v>200</v>
       </c>
       <c r="N28" t="n">
-        <v>200</v>
+        <v>16271.095</v>
       </c>
       <c r="O28" t="n">
-        <v>16271.095</v>
+        <v>0.02067185009610192</v>
       </c>
       <c r="P28" t="n">
-        <v>0.02067185009610192</v>
-      </c>
-      <c r="Q28" t="n">
         <v>3254.219</v>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
       </c>
     </row>
     <row r="29">
@@ -2418,27 +2138,17 @@
       <c r="L29" t="n">
         <v>3102.876</v>
       </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
+      <c r="M29" t="n">
+        <v>10</v>
       </c>
       <c r="N29" t="n">
-        <v>10</v>
+        <v>233303.6</v>
       </c>
       <c r="O29" t="n">
-        <v>233303.6</v>
+        <v>0.01482019816761234</v>
       </c>
       <c r="P29" t="n">
-        <v>0.01482019816761234</v>
-      </c>
-      <c r="Q29" t="n">
         <v>2333.036</v>
-      </c>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
       </c>
     </row>
     <row r="30">
@@ -2480,27 +2190,17 @@
       <c r="L30" t="n">
         <v>2159.069</v>
       </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M30" t="n">
+        <v>410</v>
       </c>
       <c r="N30" t="n">
-        <v>410</v>
+        <v>5310.329268292683</v>
       </c>
       <c r="O30" t="n">
-        <v>5310.329268292683</v>
+        <v>0.01383049989689891</v>
       </c>
       <c r="P30" t="n">
-        <v>0.01383049989689891</v>
-      </c>
-      <c r="Q30" t="n">
         <v>2177.235</v>
-      </c>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="31">
@@ -2542,27 +2242,17 @@
       <c r="L31" t="n">
         <v>2110.437</v>
       </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>Elementwise</t>
-        </is>
+      <c r="M31" t="n">
+        <v>56</v>
       </c>
       <c r="N31" t="n">
-        <v>56</v>
+        <v>37072.05357142857</v>
       </c>
       <c r="O31" t="n">
-        <v>37072.05357142857</v>
+        <v>0.01318764481255286</v>
       </c>
       <c r="P31" t="n">
-        <v>0.01318764481255286</v>
-      </c>
-      <c r="Q31" t="n">
         <v>2076.035</v>
-      </c>
-      <c r="R31" t="inlineStr">
-        <is>
-          <t>Elementwise</t>
-        </is>
       </c>
     </row>
     <row r="32">
@@ -2604,27 +2294,17 @@
       <c r="L32" t="n">
         <v>1642.067</v>
       </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
+      <c r="M32" t="n">
+        <v>10</v>
       </c>
       <c r="N32" t="n">
-        <v>10</v>
+        <v>172434.7</v>
       </c>
       <c r="O32" t="n">
-        <v>172434.7</v>
+        <v>0.01095360905263692</v>
       </c>
       <c r="P32" t="n">
-        <v>0.01095360905263692</v>
-      </c>
-      <c r="Q32" t="n">
         <v>1724.347</v>
-      </c>
-      <c r="R32" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
       </c>
     </row>
     <row r="33">
@@ -2666,27 +2346,17 @@
       <c r="L33" t="n">
         <v>1507.669</v>
       </c>
-      <c r="M33" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
+      <c r="M33" t="n">
+        <v>10</v>
       </c>
       <c r="N33" t="n">
-        <v>10</v>
+        <v>144006.4</v>
       </c>
       <c r="O33" t="n">
-        <v>144006.4</v>
+        <v>0.009147751622368659</v>
       </c>
       <c r="P33" t="n">
-        <v>0.009147751622368659</v>
-      </c>
-      <c r="Q33" t="n">
         <v>1440.064</v>
-      </c>
-      <c r="R33" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
       </c>
     </row>
     <row r="34">
@@ -2728,27 +2398,17 @@
       <c r="L34" t="n">
         <v>1080.459</v>
       </c>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>Memory</t>
-        </is>
+      <c r="M34" t="n">
+        <v>25</v>
       </c>
       <c r="N34" t="n">
-        <v>25</v>
+        <v>40373.4</v>
       </c>
       <c r="O34" t="n">
-        <v>40373.4</v>
+        <v>0.006411621902751177</v>
       </c>
       <c r="P34" t="n">
-        <v>0.006411621902751177</v>
-      </c>
-      <c r="Q34" t="n">
         <v>1009.335</v>
-      </c>
-      <c r="R34" t="inlineStr">
-        <is>
-          <t>Memory</t>
-        </is>
       </c>
     </row>
     <row r="35">
@@ -2790,27 +2450,17 @@
       <c r="L35" t="n">
         <v>929.495</v>
       </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
+      <c r="M35" t="n">
+        <v>10</v>
       </c>
       <c r="N35" t="n">
-        <v>10</v>
+        <v>92385.2</v>
       </c>
       <c r="O35" t="n">
-        <v>92385.2</v>
+        <v>0.005868606278490769</v>
       </c>
       <c r="P35" t="n">
-        <v>0.005868606278490769</v>
-      </c>
-      <c r="Q35" t="n">
         <v>923.852</v>
-      </c>
-      <c r="R35" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
       </c>
     </row>
     <row r="36">
@@ -2852,27 +2502,17 @@
       <c r="L36" t="n">
         <v>689.2910000000001</v>
       </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
+      <c r="M36" t="n">
+        <v>10</v>
       </c>
       <c r="N36" t="n">
-        <v>10</v>
+        <v>70041.10000000001</v>
       </c>
       <c r="O36" t="n">
-        <v>70041.10000000001</v>
+        <v>0.004449236882232217</v>
       </c>
       <c r="P36" t="n">
-        <v>0.004449236882232217</v>
-      </c>
-      <c r="Q36" t="n">
         <v>700.4109999999999</v>
-      </c>
-      <c r="R36" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
       </c>
     </row>
     <row r="37">
@@ -2914,27 +2554,17 @@
       <c r="L37" t="n">
         <v>486.129</v>
       </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M37" t="n">
+        <v>10</v>
       </c>
       <c r="N37" t="n">
-        <v>10</v>
+        <v>47840.9</v>
       </c>
       <c r="O37" t="n">
-        <v>47840.9</v>
+        <v>0.003039008478724396</v>
       </c>
       <c r="P37" t="n">
-        <v>0.003039008478724396</v>
-      </c>
-      <c r="Q37" t="n">
         <v>478.409</v>
-      </c>
-      <c r="R37" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="38">
@@ -2976,27 +2606,17 @@
       <c r="L38" t="n">
         <v>375.926</v>
       </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M38" t="n">
+        <v>10</v>
       </c>
       <c r="N38" t="n">
-        <v>10</v>
+        <v>37688.5</v>
       </c>
       <c r="O38" t="n">
-        <v>37688.5</v>
+        <v>0.002394095241736765</v>
       </c>
       <c r="P38" t="n">
-        <v>0.002394095241736765</v>
-      </c>
-      <c r="Q38" t="n">
         <v>376.885</v>
-      </c>
-      <c r="R38" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="39">
@@ -3038,27 +2658,17 @@
       <c r="L39" t="n">
         <v>122.522</v>
       </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>Elementwise</t>
-        </is>
+      <c r="M39" t="n">
+        <v>10</v>
       </c>
       <c r="N39" t="n">
-        <v>10</v>
+        <v>12236.1</v>
       </c>
       <c r="O39" t="n">
-        <v>12236.1</v>
+        <v>0.0007772765906686449</v>
       </c>
       <c r="P39" t="n">
-        <v>0.0007772765906686449</v>
-      </c>
-      <c r="Q39" t="n">
         <v>122.361</v>
-      </c>
-      <c r="R39" t="inlineStr">
-        <is>
-          <t>Elementwise</t>
-        </is>
       </c>
     </row>
     <row r="40">
@@ -3100,27 +2710,17 @@
       <c r="L40" t="n">
         <v>88.842</v>
       </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M40" t="n">
+        <v>20</v>
       </c>
       <c r="N40" t="n">
-        <v>20</v>
+        <v>4384</v>
       </c>
       <c r="O40" t="n">
-        <v>4384</v>
+        <v>0.0005569716778207664</v>
       </c>
       <c r="P40" t="n">
-        <v>0.0005569716778207664</v>
-      </c>
-      <c r="Q40" t="n">
         <v>87.68000000000001</v>
-      </c>
-      <c r="R40" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="41">
@@ -3162,27 +2762,17 @@
       <c r="L41" t="n">
         <v>80.322</v>
       </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M41" t="n">
+        <v>10</v>
       </c>
       <c r="N41" t="n">
-        <v>10</v>
+        <v>7772</v>
       </c>
       <c r="O41" t="n">
-        <v>7772</v>
+        <v>0.0004937025410610169</v>
       </c>
       <c r="P41" t="n">
-        <v>0.0004937025410610169</v>
-      </c>
-      <c r="Q41" t="n">
         <v>77.72</v>
-      </c>
-      <c r="R41" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="42">
@@ -3224,27 +2814,17 @@
       <c r="L42" t="n">
         <v>57.681</v>
       </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>Normalization</t>
-        </is>
+      <c r="M42" t="n">
+        <v>10</v>
       </c>
       <c r="N42" t="n">
-        <v>10</v>
+        <v>5712.1</v>
       </c>
       <c r="O42" t="n">
-        <v>5712.1</v>
+        <v>0.0003628510402463503</v>
       </c>
       <c r="P42" t="n">
-        <v>0.0003628510402463503</v>
-      </c>
-      <c r="Q42" t="n">
         <v>57.121</v>
-      </c>
-      <c r="R42" t="inlineStr">
-        <is>
-          <t>Normalization</t>
-        </is>
       </c>
     </row>
     <row r="43">
@@ -3286,27 +2866,17 @@
       <c r="L43" t="n">
         <v>56.96</v>
       </c>
-      <c r="M43" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M43" t="n">
+        <v>10</v>
       </c>
       <c r="N43" t="n">
-        <v>10</v>
+        <v>5696.3</v>
       </c>
       <c r="O43" t="n">
-        <v>5696.3</v>
+        <v>0.0003618473732174306</v>
       </c>
       <c r="P43" t="n">
-        <v>0.0003618473732174306</v>
-      </c>
-      <c r="Q43" t="n">
         <v>56.963</v>
-      </c>
-      <c r="R43" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="44">
@@ -3348,27 +2918,17 @@
       <c r="L44" t="n">
         <v>50.361</v>
       </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M44" t="n">
+        <v>10</v>
       </c>
       <c r="N44" t="n">
-        <v>10</v>
+        <v>4804.1</v>
       </c>
       <c r="O44" t="n">
-        <v>4804.1</v>
+        <v>0.0003051719476983056</v>
       </c>
       <c r="P44" t="n">
-        <v>0.0003051719476983056</v>
-      </c>
-      <c r="Q44" t="n">
         <v>48.041</v>
-      </c>
-      <c r="R44" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="45">
@@ -3410,27 +2970,17 @@
       <c r="L45" t="n">
         <v>42.921</v>
       </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M45" t="n">
+        <v>10</v>
       </c>
       <c r="N45" t="n">
-        <v>10</v>
+        <v>4344.1</v>
       </c>
       <c r="O45" t="n">
-        <v>4344.1</v>
+        <v>0.0002759512620462125</v>
       </c>
       <c r="P45" t="n">
-        <v>0.0002759512620462125</v>
-      </c>
-      <c r="Q45" t="n">
         <v>43.441</v>
-      </c>
-      <c r="R45" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="46">
@@ -3472,27 +3022,17 @@
       <c r="L46" t="n">
         <v>42.28</v>
       </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M46" t="n">
+        <v>10</v>
       </c>
       <c r="N46" t="n">
-        <v>10</v>
+        <v>4344</v>
       </c>
       <c r="O46" t="n">
-        <v>4344</v>
+        <v>0.0002759449097232446</v>
       </c>
       <c r="P46" t="n">
-        <v>0.0002759449097232446</v>
-      </c>
-      <c r="Q46" t="n">
         <v>43.44</v>
-      </c>
-      <c r="R46" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
     <row r="47">
@@ -3534,27 +3074,17 @@
       <c r="L47" t="n">
         <v>41.08</v>
       </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
+      <c r="M47" t="n">
+        <v>10</v>
       </c>
       <c r="N47" t="n">
-        <v>10</v>
+        <v>4252</v>
       </c>
       <c r="O47" t="n">
-        <v>4252</v>
+        <v>0.000270100772592826</v>
       </c>
       <c r="P47" t="n">
-        <v>0.000270100772592826</v>
-      </c>
-      <c r="Q47" t="n">
         <v>42.52</v>
-      </c>
-      <c r="R47" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>